<commit_message>
Creating the diffusion matrix, A.
</commit_message>
<xml_diff>
--- a/NE5002Project/Data/input.xlsx
+++ b/NE5002Project/Data/input.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xanderbard/Documents/GitHub/NE5002Project/NE5002Project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE755290-847C-D646-8F8B-5B49DF14CA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63ED6CA0-3739-D842-B805-407515F46D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="500" windowWidth="12800" windowHeight="19940" xr2:uid="{8F394183-57D9-494C-8342-290491876281}"/>
+    <workbookView xWindow="22920" yWindow="500" windowWidth="22960" windowHeight="27140" xr2:uid="{8F394183-57D9-494C-8342-290491876281}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>X-start</t>
   </si>
@@ -48,12 +48,6 @@
   </si>
   <si>
     <t>CS-s</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>Density</t>
   </si>
   <si>
     <t>Material 1</t>
@@ -101,9 +95,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,20 +413,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16055E6E-9EC4-AB4B-867B-E423287A8AE6}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -455,51 +450,29 @@
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1">
-        <v>7</v>
+      <c r="B4" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1">
-        <v>10</v>
+      <c r="B5" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Good progress on matrix builder
Need to fix absorption cross section calculations
</commit_message>
<xml_diff>
--- a/NE5002Project/Data/input.xlsx
+++ b/NE5002Project/Data/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xanderbard/Documents/GitHub/NE5002Project/NE5002Project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63ED6CA0-3739-D842-B805-407515F46D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB895C9-CFCE-BF4C-BBBF-6FC8CE6AC470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22920" yWindow="500" windowWidth="22960" windowHeight="27140" xr2:uid="{8F394183-57D9-494C-8342-290491876281}"/>
   </bookViews>
@@ -416,7 +416,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -461,7 +461,7 @@
         <v>0.5</v>
       </c>
       <c r="C4" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -472,7 +472,7 @@
         <v>0.5</v>
       </c>
       <c r="C5" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Great progress torward matrix.
Last steps: Recursion, solver, and graphs
</commit_message>
<xml_diff>
--- a/NE5002Project/Data/input.xlsx
+++ b/NE5002Project/Data/input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xanderbard/Documents/GitHub/NE5002Project/NE5002Project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB895C9-CFCE-BF4C-BBBF-6FC8CE6AC470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C75FC9-37A5-FC47-9B89-54365EB2E2B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22920" yWindow="500" windowWidth="22960" windowHeight="27140" xr2:uid="{8F394183-57D9-494C-8342-290491876281}"/>
   </bookViews>
@@ -416,7 +416,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
12/3 Start of Day
</commit_message>
<xml_diff>
--- a/NE5002Project/Data/input.xlsx
+++ b/NE5002Project/Data/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xanderbard/Documents/GitHub/NE5002Project/NE5002Project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C75FC9-37A5-FC47-9B89-54365EB2E2B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0CD3C2-E916-044E-B17E-B44383663179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22920" yWindow="500" windowWidth="22960" windowHeight="27140" xr2:uid="{8F394183-57D9-494C-8342-290491876281}"/>
   </bookViews>
@@ -439,7 +439,7 @@
       </c>
       <c r="C2">
         <f>B3</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -447,10 +447,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="1">
         <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Final code (i think)
</commit_message>
<xml_diff>
--- a/NE5002Project/Data/input.xlsx
+++ b/NE5002Project/Data/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xanderbard/Documents/GitHub/NE5002Project/NE5002Project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1909414D-DF96-7645-94D9-59A144AD2F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{146101AD-0C7D-A641-AFDB-1A301304ADA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="22940" windowHeight="27140" xr2:uid="{8F394183-57D9-494C-8342-290491876281}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22940" windowHeight="27160" xr2:uid="{8F394183-57D9-494C-8342-290491876281}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -416,7 +416,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -439,7 +439,7 @@
       </c>
       <c r="C2">
         <f>B3</f>
-        <v>1</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -447,10 +447,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C3" s="1">
         <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -473,7 +473,7 @@
         <v>0.45</v>
       </c>
       <c r="C5" s="2">
-        <f>0.9*C4</f>
+        <f>C4*0.9</f>
         <v>0.45</v>
       </c>
     </row>

</xml_diff>